<commit_message>
hoan thanh tinh luong
</commit_message>
<xml_diff>
--- a/assets/SourceFile/chamcong_t06_2022.xlsx
+++ b/assets/SourceFile/chamcong_t06_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Mã NV</t>
   </si>
@@ -32,10 +32,13 @@
     <t>x</t>
   </si>
   <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
     <t>Hà Quốc Huy</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>Trịnh Thành Công</t>
@@ -142,7 +145,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0"/>
+      <border/>
+    </dxf>
     <dxf>
       <font>
         <sz val="10"/>
@@ -454,7 +470,7 @@
   <dimension ref="A1:AH22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>4</v>
@@ -617,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>4</v>
@@ -629,11 +645,26 @@
         <v>4</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH2" s="1">
         <f>COUNTIF(C2:AG2, "x")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -641,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -656,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>4</v>
@@ -677,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>4</v>
@@ -689,11 +720,26 @@
         <v>4</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH3" s="1">
         <f>COUNTIF(C3:AG3, "x")</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -701,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -716,7 +762,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>6</v>
@@ -737,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>6</v>
@@ -751,9 +797,24 @@
       <c r="R4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="S4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="AH4" s="1">
         <f>COUNTIF(C4:AG4, "x")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -761,7 +822,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -776,7 +837,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>4</v>
@@ -797,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>6</v>
@@ -811,9 +872,24 @@
       <c r="R5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="S5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="AH5" s="1">
         <f>COUNTIF(C5:AG5, "x")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -821,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -836,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>4</v>
@@ -857,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>4</v>
@@ -871,9 +947,24 @@
       <c r="R6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="S6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="AH6" s="1">
         <f>COUNTIF(C6:AG6, "x")</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -881,7 +972,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -896,7 +987,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>4</v>
@@ -917,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>4</v>
@@ -929,11 +1020,26 @@
         <v>4</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH7" s="1">
         <f>COUNTIF(C7:AG7, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:34">
@@ -941,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -956,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>4</v>
@@ -977,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>4</v>
@@ -989,11 +1095,26 @@
         <v>4</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="W8" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH8" s="1">
         <f>COUNTIF(C8:AG8, "x")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -1001,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1016,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>4</v>
@@ -1037,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>4</v>
@@ -1049,11 +1170,26 @@
         <v>4</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W9" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH9" s="1">
         <f>COUNTIF(C9:AG9, "x")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -1061,7 +1197,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1076,7 +1212,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>4</v>
@@ -1097,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>4</v>
@@ -1109,11 +1245,26 @@
         <v>4</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W10" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH10" s="1">
         <f>COUNTIF(C10:AG10, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -1121,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -1136,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>4</v>
@@ -1157,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>4</v>
@@ -1169,11 +1320,26 @@
         <v>4</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W11" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH11" s="1">
         <f>COUNTIF(C11:AG11, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -1181,7 +1347,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
@@ -1196,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>4</v>
@@ -1217,7 +1383,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>6</v>
@@ -1231,9 +1397,24 @@
       <c r="R12" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="S12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="AH12" s="1">
         <f>COUNTIF(C12:AG12, "x")</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:34">
@@ -1241,7 +1422,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
@@ -1256,7 +1437,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>4</v>
@@ -1277,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>4</v>
@@ -1289,11 +1470,26 @@
         <v>4</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH13" s="1">
         <f>COUNTIF(C13:AG13, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:34">
@@ -1301,7 +1497,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>4</v>
@@ -1316,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>6</v>
@@ -1337,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>4</v>
@@ -1349,11 +1545,26 @@
         <v>4</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH14" s="1">
         <f>COUNTIF(C14:AG14, "x")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -1361,7 +1572,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -1376,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>6</v>
@@ -1397,7 +1608,7 @@
         <v>4</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>4</v>
@@ -1409,11 +1620,26 @@
         <v>4</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH15" s="1">
         <f>COUNTIF(C15:AG15, "x")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -1421,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1436,7 +1662,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>4</v>
@@ -1457,7 +1683,7 @@
         <v>4</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>4</v>
@@ -1469,11 +1695,26 @@
         <v>4</v>
       </c>
       <c r="R16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH16" s="1">
         <f>COUNTIF(C16:AG16, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -1481,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -1496,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>4</v>
@@ -1517,7 +1758,7 @@
         <v>4</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>4</v>
@@ -1529,11 +1770,26 @@
         <v>4</v>
       </c>
       <c r="R17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH17" s="1">
         <f>COUNTIF(C17:AG17, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -1541,7 +1797,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
@@ -1556,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>4</v>
@@ -1577,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>4</v>
@@ -1589,11 +1845,26 @@
         <v>4</v>
       </c>
       <c r="R18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH18" s="1">
         <f>COUNTIF(C18:AG18, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:34">
@@ -1601,7 +1872,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1616,7 +1887,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>4</v>
@@ -1637,7 +1908,7 @@
         <v>4</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>4</v>
@@ -1649,11 +1920,26 @@
         <v>4</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH19" s="1">
         <f>COUNTIF(C19:AG19, "x")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:34">
@@ -1661,7 +1947,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -1676,7 +1962,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>4</v>
@@ -1697,7 +1983,7 @@
         <v>4</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>4</v>
@@ -1709,11 +1995,26 @@
         <v>4</v>
       </c>
       <c r="R20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V20" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W20" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH20" s="1">
         <f>COUNTIF(C20:AG20, "x")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:34">
@@ -1721,7 +2022,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1736,7 +2037,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>4</v>
@@ -1757,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>4</v>
@@ -1769,11 +2070,26 @@
         <v>4</v>
       </c>
       <c r="R21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V21" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W21" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH21" s="1">
         <f>COUNTIF(C21:AG21, "x")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:34">
@@ -1781,14 +2097,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W22" s="0" t="s">
         <v>4</v>
       </c>
       <c r="AH22" s="0">
         <f>COUNTIF(C22:AG22, "x")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1798,9 +2129,9 @@
       <formula>"v"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:XFD20">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"v"</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"CN"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>